<commit_message>
Ajustes para Coligada SESI
</commit_message>
<xml_diff>
--- a/models/Responsáveis Unidade.xlsx
+++ b/models/Responsáveis Unidade.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jangelica\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbravo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{3FCEDBBA-3073-409B-89AC-F1FE794A0045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E3C9CE9-B4A8-4A4E-8F39-81E3AD2B5154}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="11_5EC6A759C5BEA9B490783A4332F7EA4E719EA68A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B78A26AC-7722-4DAD-BA39-C06A9D849924}"/>
+  <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7476" windowHeight="7752" xr2:uid="{F38AC101-A357-45A6-B271-E59CE9F06B73}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="4930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -53,6 +54,9 @@
     <t>Responsáveis ADM3</t>
   </si>
   <si>
+    <t>Responsáveis ADM4</t>
+  </si>
+  <si>
     <t>CENTRO DE EDUCAÇÃO E TECNOLOGIA ARIVALDO SILVEIRA FONTES</t>
   </si>
   <si>
@@ -68,13 +72,7 @@
     <t>CENTRO DE EDUCAÇÃO PROFISSIONAL JONES DOS SANTOS NEVES</t>
   </si>
   <si>
-    <t>gavieira@senai-es.org.br</t>
-  </si>
-  <si>
-    <t>jmazini@findes.org.br</t>
-  </si>
-  <si>
-    <t>nviana@findes.org.br</t>
+    <t>wescleydecarvalho@hotmail.com</t>
   </si>
   <si>
     <t>CENTRO DE EDUCAÇÃO PROFISSIONAL HÉLCIO REZENDE DIAS</t>
@@ -96,6 +94,9 @@
   </si>
   <si>
     <t>CENTRO DE EDUCAÇÃO PROFISSIONAL EURICO DE AGUIAR SALLES</t>
+  </si>
+  <si>
+    <t>wssilva@findes.org.br</t>
   </si>
   <si>
     <t>CENTRO DE EDUCAÇÃO PROFISSIONAL ALBANO FRANCO</t>
@@ -159,7 +160,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -167,26 +168,51 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -501,178 +527,209 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A5BCACD-1A01-4721-987F-6E3CAB7CCFA8}">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="10.28515625" customWidth="1"/>
     <col min="2" max="2" width="61.7109375" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="23.85546875" customWidth="1"/>
     <col min="5" max="5" width="24.85546875" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1">
+    <row r="2" spans="1:6">
+      <c r="A2" s="2">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="2">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="2">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="B5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="2">
         <v>7</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="2">
         <v>8</v>
       </c>
+      <c r="B7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
+    <row r="8" spans="1:6">
+      <c r="A8" s="2">
         <v>9</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="B8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="2">
         <v>10</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="B9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="1">
-        <v>7</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="1">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="1">
-        <v>9</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="1">
-        <v>10</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="1">
-        <v>12</v>
-      </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="7" t="s">
         <v>27</v>
       </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{388119B9-3188-4101-9334-528E6BC2ADA7}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{E8515EC7-0B47-4BB8-8995-B0B2A4118263}"/>
-    <hyperlink ref="D3" r:id="rId3" xr:uid="{5264F981-F56E-4089-8152-A23F49C02ACB}"/>
-    <hyperlink ref="C4" r:id="rId4" xr:uid="{CE023999-AC69-47DA-9F8C-3E349C0D0FAD}"/>
-    <hyperlink ref="E4" r:id="rId5" xr:uid="{7E34C4C1-0491-4D3E-839C-ECCE26C3DB2B}"/>
-    <hyperlink ref="C5" r:id="rId6" xr:uid="{5B1A0CCE-2FF7-49A2-A611-F1B085EA2E70}"/>
-    <hyperlink ref="C9" r:id="rId7" xr:uid="{1C77848B-7FC6-46A3-A813-6140B59ECD65}"/>
-    <hyperlink ref="C7" r:id="rId8" xr:uid="{C791C3C8-FCDC-4E38-BDAD-15933C0DAF1F}"/>
-    <hyperlink ref="C8" r:id="rId9" xr:uid="{F6499BE5-664C-48E7-B889-B30F24B05FB0}"/>
-    <hyperlink ref="D10" r:id="rId10" xr:uid="{E71D4E37-C48D-4420-BC9C-B3131BCB5B51}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C5" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C9" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C7" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="C8" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="D10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="8d55533a-b699-46c7-bc49-e3db65ffe96c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d594eb50-3db9-40f8-b797-706e4a5c3347">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100FD92C8847C016442B6B2FCBB244BFE1B" ma:contentTypeVersion="11" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="a84a73879ab9dfec17d55bd241ff31c0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d594eb50-3db9-40f8-b797-706e4a5c3347" xmlns:ns3="8d55533a-b699-46c7-bc49-e3db65ffe96c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f53b5becae0d7122eef7e7b40a85c9a2" ns2:_="" ns3:_="">
     <xsd:import namespace="d594eb50-3db9-40f8-b797-706e4a5c3347"/>
@@ -867,17 +924,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="8d55533a-b699-46c7-bc49-e3db65ffe96c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d594eb50-3db9-40f8-b797-706e4a5c3347">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -888,11 +934,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6248EC5D-F447-4CBC-A58A-E5522C04D31E}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E73C2EDF-A3C0-451C-B5AB-90DBB7808637}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6248EC5D-F447-4CBC-A58A-E5522C04D31E}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>